<commit_message>
Completed Feature ID's CS, MAXS, and RCPT
</commit_message>
<xml_diff>
--- a/P11/Scrum_MICE_Sprint_5.xlsx
+++ b/P11/Scrum_MICE_Sprint_5.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="220">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -1206,10 +1206,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822405395279131"/>
-          <c:y val="0.161875945537065"/>
-          <c:w val="0.884351192706382"/>
-          <c:h val="0.63565305093293"/>
+          <c:x val="0.0822456753887466"/>
+          <c:y val="0.161896356071113"/>
+          <c:w val="0.884281521263973"/>
+          <c:h val="0.635607111335267"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1318,11 +1318,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16766130"/>
-        <c:axId val="65212371"/>
+        <c:axId val="3042615"/>
+        <c:axId val="37887512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16766130"/>
+        <c:axId val="3042615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1389,12 +1389,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65212371"/>
+        <c:crossAx val="37887512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65212371"/>
+        <c:axId val="37887512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1469,7 +1469,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16766130"/>
+        <c:crossAx val="3042615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1489,7 +1489,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1624,11 +1624,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="11544727"/>
-        <c:axId val="28252349"/>
+        <c:axId val="91226596"/>
+        <c:axId val="5972716"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="11544727"/>
+        <c:axId val="91226596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1693,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28252349"/>
+        <c:crossAx val="5972716"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1701,7 +1701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28252349"/>
+        <c:axId val="5972716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,7 +1775,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11544727"/>
+        <c:crossAx val="91226596"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1795,7 +1795,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1930,11 +1930,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="34674930"/>
-        <c:axId val="50393324"/>
+        <c:axId val="15209356"/>
+        <c:axId val="67439798"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="34674930"/>
+        <c:axId val="15209356"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +1999,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50393324"/>
+        <c:crossAx val="67439798"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2007,7 +2007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50393324"/>
+        <c:axId val="67439798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2081,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34674930"/>
+        <c:crossAx val="15209356"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2101,7 +2101,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2236,11 +2236,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="48107833"/>
-        <c:axId val="21065689"/>
+        <c:axId val="26623412"/>
+        <c:axId val="82430155"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48107833"/>
+        <c:axId val="26623412"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2305,7 +2305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21065689"/>
+        <c:crossAx val="82430155"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2313,7 +2313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="21065689"/>
+        <c:axId val="82430155"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2387,7 +2387,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48107833"/>
+        <c:crossAx val="26623412"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2407,7 +2407,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2542,11 +2542,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="69154053"/>
-        <c:axId val="96706523"/>
+        <c:axId val="23676919"/>
+        <c:axId val="26832876"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69154053"/>
+        <c:axId val="23676919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,7 +2611,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96706523"/>
+        <c:crossAx val="26832876"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2619,7 +2619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96706523"/>
+        <c:axId val="26832876"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2693,7 +2693,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69154053"/>
+        <c:crossAx val="23676919"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2713,7 +2713,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2830,10 +2830,10 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2848,11 +2848,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="85042073"/>
-        <c:axId val="63652676"/>
+        <c:axId val="30487926"/>
+        <c:axId val="62234585"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85042073"/>
+        <c:axId val="30487926"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,7 +2917,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63652676"/>
+        <c:crossAx val="62234585"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2925,7 +2925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63652676"/>
+        <c:axId val="62234585"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2999,7 +2999,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85042073"/>
+        <c:crossAx val="30487926"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3019,7 +3019,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -3154,11 +3154,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="46894238"/>
-        <c:axId val="83117076"/>
+        <c:axId val="71479420"/>
+        <c:axId val="67462817"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46894238"/>
+        <c:axId val="71479420"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3223,7 +3223,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83117076"/>
+        <c:crossAx val="67462817"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3231,7 +3231,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83117076"/>
+        <c:axId val="67462817"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3305,7 +3305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46894238"/>
+        <c:crossAx val="71479420"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3325,7 +3325,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -3343,9 +3343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3202200</xdr:colOff>
+      <xdr:colOff>3201840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3353,8 +3353,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9118080" y="268200"/>
-        <a:ext cx="5764680" cy="2855160"/>
+        <a:off x="9116280" y="268200"/>
+        <a:ext cx="5764320" cy="2854800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3378,9 +3378,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3388,8 +3388,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3413,9 +3413,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3423,8 +3423,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3448,9 +3448,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3458,8 +3458,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3483,9 +3483,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3493,8 +3493,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3518,9 +3518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3528,8 +3528,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3553,9 +3553,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3563,8 +3563,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3594,11 +3594,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="39.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="53.71"/>
@@ -5697,7 +5697,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6679,7 +6679,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7656,7 +7656,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8651,7 +8651,7 @@
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9633,7 +9633,7 @@
       <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9815,11 +9815,11 @@
       </c>
       <c r="B13" s="28" t="n">
         <f aca="false">B12-C13</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="28" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
@@ -9831,7 +9831,7 @@
       </c>
       <c r="B14" s="28" t="n">
         <f aca="false">B13-C14</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="28" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -9893,7 +9893,9 @@
       <c r="D18" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="38" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -9905,7 +9907,9 @@
       <c r="D19" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="40"/>
+      <c r="E19" s="38" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -9917,7 +9921,9 @@
       <c r="D20" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="40"/>
+      <c r="E20" s="38" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -9929,7 +9935,9 @@
       <c r="D21" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="40"/>
+      <c r="E21" s="38" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -9941,7 +9949,9 @@
       <c r="D22" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="40"/>
+      <c r="E22" s="38" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -9949,7 +9959,7 @@
       </c>
       <c r="B23" s="39"/>
       <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -9957,7 +9967,7 @@
       </c>
       <c r="B24" s="39"/>
       <c r="D24" s="39"/>
-      <c r="E24" s="40"/>
+      <c r="E24" s="38"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -9965,7 +9975,7 @@
       </c>
       <c r="B25" s="39"/>
       <c r="D25" s="39"/>
-      <c r="E25" s="40"/>
+      <c r="E25" s="38"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -9973,7 +9983,7 @@
       </c>
       <c r="B26" s="39"/>
       <c r="D26" s="39"/>
-      <c r="E26" s="40"/>
+      <c r="E26" s="38"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -9981,7 +9991,7 @@
       </c>
       <c r="B27" s="39"/>
       <c r="D27" s="39"/>
-      <c r="E27" s="40"/>
+      <c r="E27" s="38"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -9989,7 +9999,7 @@
       </c>
       <c r="B28" s="39"/>
       <c r="D28" s="39"/>
-      <c r="E28" s="40"/>
+      <c r="E28" s="38"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -9997,7 +10007,7 @@
       </c>
       <c r="B29" s="39"/>
       <c r="D29" s="39"/>
-      <c r="E29" s="40"/>
+      <c r="E29" s="38"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -10005,7 +10015,7 @@
       </c>
       <c r="B30" s="39"/>
       <c r="D30" s="39"/>
-      <c r="E30" s="40"/>
+      <c r="E30" s="38"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -10013,7 +10023,7 @@
       </c>
       <c r="B31" s="39"/>
       <c r="D31" s="39"/>
-      <c r="E31" s="40"/>
+      <c r="E31" s="38"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -10021,7 +10031,7 @@
       </c>
       <c r="B32" s="39"/>
       <c r="D32" s="39"/>
-      <c r="E32" s="40"/>
+      <c r="E32" s="38"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -10029,7 +10039,7 @@
       </c>
       <c r="B33" s="39"/>
       <c r="D33" s="39"/>
-      <c r="E33" s="40"/>
+      <c r="E33" s="38"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -10037,7 +10047,7 @@
       </c>
       <c r="B34" s="39"/>
       <c r="D34" s="39"/>
-      <c r="E34" s="40"/>
+      <c r="E34" s="38"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -10045,7 +10055,7 @@
       </c>
       <c r="B35" s="39"/>
       <c r="D35" s="39"/>
-      <c r="E35" s="40"/>
+      <c r="E35" s="38"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -10053,7 +10063,7 @@
       </c>
       <c r="B36" s="39"/>
       <c r="D36" s="39"/>
-      <c r="E36" s="40"/>
+      <c r="E36" s="38"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -10061,7 +10071,7 @@
       </c>
       <c r="B37" s="39"/>
       <c r="D37" s="39"/>
-      <c r="E37" s="40"/>
+      <c r="E37" s="38"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -10069,7 +10079,7 @@
       </c>
       <c r="B38" s="39"/>
       <c r="D38" s="39"/>
-      <c r="E38" s="40"/>
+      <c r="E38" s="38"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -10077,7 +10087,7 @@
       </c>
       <c r="B39" s="39"/>
       <c r="D39" s="39"/>
-      <c r="E39" s="40"/>
+      <c r="E39" s="38"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -10085,7 +10095,7 @@
       </c>
       <c r="B40" s="39"/>
       <c r="D40" s="39"/>
-      <c r="E40" s="40"/>
+      <c r="E40" s="38"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -10093,7 +10103,7 @@
       </c>
       <c r="B41" s="39"/>
       <c r="D41" s="39"/>
-      <c r="E41" s="40"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -10101,7 +10111,7 @@
       </c>
       <c r="B42" s="39"/>
       <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
+      <c r="E42" s="38"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -10109,7 +10119,7 @@
       </c>
       <c r="B43" s="39"/>
       <c r="D43" s="39"/>
-      <c r="E43" s="40"/>
+      <c r="E43" s="38"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -10117,7 +10127,7 @@
       </c>
       <c r="B44" s="39"/>
       <c r="D44" s="39"/>
-      <c r="E44" s="40"/>
+      <c r="E44" s="38"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -10125,7 +10135,7 @@
       </c>
       <c r="B45" s="39"/>
       <c r="D45" s="39"/>
-      <c r="E45" s="40"/>
+      <c r="E45" s="38"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -10133,7 +10143,7 @@
       </c>
       <c r="B46" s="39"/>
       <c r="D46" s="39"/>
-      <c r="E46" s="40"/>
+      <c r="E46" s="38"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -10141,7 +10151,7 @@
       </c>
       <c r="B47" s="39"/>
       <c r="D47" s="39"/>
-      <c r="E47" s="40"/>
+      <c r="E47" s="38"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -10149,7 +10159,7 @@
       </c>
       <c r="B48" s="39"/>
       <c r="D48" s="39"/>
-      <c r="E48" s="40"/>
+      <c r="E48" s="38"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -10157,7 +10167,7 @@
       </c>
       <c r="B49" s="39"/>
       <c r="D49" s="39"/>
-      <c r="E49" s="40"/>
+      <c r="E49" s="38"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -10165,7 +10175,7 @@
       </c>
       <c r="B50" s="39"/>
       <c r="D50" s="39"/>
-      <c r="E50" s="40"/>
+      <c r="E50" s="38"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -10173,7 +10183,7 @@
       </c>
       <c r="B51" s="39"/>
       <c r="D51" s="39"/>
-      <c r="E51" s="40"/>
+      <c r="E51" s="38"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -10181,7 +10191,7 @@
       </c>
       <c r="B52" s="39"/>
       <c r="D52" s="39"/>
-      <c r="E52" s="40"/>
+      <c r="E52" s="38"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -10189,7 +10199,7 @@
       </c>
       <c r="B53" s="39"/>
       <c r="D53" s="39"/>
-      <c r="E53" s="40"/>
+      <c r="E53" s="38"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -10197,7 +10207,7 @@
       </c>
       <c r="B54" s="39"/>
       <c r="D54" s="39"/>
-      <c r="E54" s="40"/>
+      <c r="E54" s="38"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -10205,7 +10215,7 @@
       </c>
       <c r="B55" s="39"/>
       <c r="D55" s="39"/>
-      <c r="E55" s="40"/>
+      <c r="E55" s="38"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -10213,7 +10223,7 @@
       </c>
       <c r="B56" s="39"/>
       <c r="D56" s="39"/>
-      <c r="E56" s="40"/>
+      <c r="E56" s="38"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -10221,7 +10231,7 @@
       </c>
       <c r="B57" s="39"/>
       <c r="D57" s="39"/>
-      <c r="E57" s="40"/>
+      <c r="E57" s="38"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -10229,7 +10239,7 @@
       </c>
       <c r="B58" s="39"/>
       <c r="D58" s="39"/>
-      <c r="E58" s="40"/>
+      <c r="E58" s="38"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -10237,7 +10247,7 @@
       </c>
       <c r="B59" s="39"/>
       <c r="D59" s="39"/>
-      <c r="E59" s="40"/>
+      <c r="E59" s="38"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -10245,7 +10255,7 @@
       </c>
       <c r="B60" s="39"/>
       <c r="D60" s="39"/>
-      <c r="E60" s="40"/>
+      <c r="E60" s="38"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -10253,7 +10263,7 @@
       </c>
       <c r="B61" s="39"/>
       <c r="D61" s="39"/>
-      <c r="E61" s="40"/>
+      <c r="E61" s="38"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -10261,7 +10271,7 @@
       </c>
       <c r="B62" s="39"/>
       <c r="D62" s="39"/>
-      <c r="E62" s="40"/>
+      <c r="E62" s="38"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -10269,7 +10279,7 @@
       </c>
       <c r="B63" s="39"/>
       <c r="D63" s="39"/>
-      <c r="E63" s="40"/>
+      <c r="E63" s="38"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -10277,7 +10287,7 @@
       </c>
       <c r="B64" s="39"/>
       <c r="D64" s="39"/>
-      <c r="E64" s="40"/>
+      <c r="E64" s="38"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -10285,7 +10295,7 @@
       </c>
       <c r="B65" s="39"/>
       <c r="D65" s="39"/>
-      <c r="E65" s="40"/>
+      <c r="E65" s="38"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -10293,7 +10303,7 @@
       </c>
       <c r="B66" s="39"/>
       <c r="D66" s="39"/>
-      <c r="E66" s="40"/>
+      <c r="E66" s="38"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
@@ -10301,7 +10311,7 @@
       </c>
       <c r="B67" s="39"/>
       <c r="D67" s="39"/>
-      <c r="E67" s="40"/>
+      <c r="E67" s="38"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
@@ -10309,7 +10319,7 @@
       </c>
       <c r="B68" s="39"/>
       <c r="D68" s="39"/>
-      <c r="E68" s="40"/>
+      <c r="E68" s="38"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
@@ -10317,7 +10327,7 @@
       </c>
       <c r="B69" s="39"/>
       <c r="D69" s="39"/>
-      <c r="E69" s="40"/>
+      <c r="E69" s="38"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -10325,7 +10335,7 @@
       </c>
       <c r="B70" s="39"/>
       <c r="D70" s="39"/>
-      <c r="E70" s="40"/>
+      <c r="E70" s="38"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
@@ -10333,7 +10343,7 @@
       </c>
       <c r="B71" s="39"/>
       <c r="D71" s="39"/>
-      <c r="E71" s="40"/>
+      <c r="E71" s="38"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
@@ -10341,7 +10351,7 @@
       </c>
       <c r="B72" s="39"/>
       <c r="D72" s="39"/>
-      <c r="E72" s="40"/>
+      <c r="E72" s="38"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
@@ -10349,7 +10359,7 @@
       </c>
       <c r="B73" s="39"/>
       <c r="D73" s="39"/>
-      <c r="E73" s="40"/>
+      <c r="E73" s="38"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
@@ -10357,7 +10367,7 @@
       </c>
       <c r="B74" s="39"/>
       <c r="D74" s="39"/>
-      <c r="E74" s="40"/>
+      <c r="E74" s="38"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
@@ -10365,7 +10375,7 @@
       </c>
       <c r="B75" s="39"/>
       <c r="D75" s="39"/>
-      <c r="E75" s="40"/>
+      <c r="E75" s="38"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
@@ -10373,7 +10383,7 @@
       </c>
       <c r="B76" s="39"/>
       <c r="D76" s="39"/>
-      <c r="E76" s="40"/>
+      <c r="E76" s="38"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
@@ -10381,7 +10391,7 @@
       </c>
       <c r="B77" s="39"/>
       <c r="D77" s="39"/>
-      <c r="E77" s="40"/>
+      <c r="E77" s="38"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
@@ -10389,7 +10399,7 @@
       </c>
       <c r="B78" s="39"/>
       <c r="D78" s="39"/>
-      <c r="E78" s="40"/>
+      <c r="E78" s="38"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
@@ -10397,7 +10407,7 @@
       </c>
       <c r="B79" s="39"/>
       <c r="D79" s="39"/>
-      <c r="E79" s="40"/>
+      <c r="E79" s="38"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
@@ -10405,7 +10415,7 @@
       </c>
       <c r="B80" s="39"/>
       <c r="D80" s="39"/>
-      <c r="E80" s="40"/>
+      <c r="E80" s="38"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
@@ -10413,7 +10423,7 @@
       </c>
       <c r="B81" s="39"/>
       <c r="D81" s="39"/>
-      <c r="E81" s="40"/>
+      <c r="E81" s="38"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
@@ -10421,7 +10431,7 @@
       </c>
       <c r="B82" s="39"/>
       <c r="D82" s="39"/>
-      <c r="E82" s="40"/>
+      <c r="E82" s="38"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
@@ -10429,7 +10439,7 @@
       </c>
       <c r="B83" s="39"/>
       <c r="D83" s="39"/>
-      <c r="E83" s="40"/>
+      <c r="E83" s="38"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
@@ -10437,7 +10447,7 @@
       </c>
       <c r="B84" s="39"/>
       <c r="D84" s="39"/>
-      <c r="E84" s="40"/>
+      <c r="E84" s="38"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
@@ -10445,7 +10455,7 @@
       </c>
       <c r="B85" s="39"/>
       <c r="D85" s="39"/>
-      <c r="E85" s="40"/>
+      <c r="E85" s="38"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
@@ -10453,7 +10463,7 @@
       </c>
       <c r="B86" s="39"/>
       <c r="D86" s="39"/>
-      <c r="E86" s="40"/>
+      <c r="E86" s="38"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
@@ -10461,7 +10471,7 @@
       </c>
       <c r="B87" s="39"/>
       <c r="D87" s="39"/>
-      <c r="E87" s="40"/>
+      <c r="E87" s="38"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
@@ -10469,7 +10479,7 @@
       </c>
       <c r="B88" s="39"/>
       <c r="D88" s="39"/>
-      <c r="E88" s="40"/>
+      <c r="E88" s="38"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
@@ -10477,7 +10487,7 @@
       </c>
       <c r="B89" s="39"/>
       <c r="D89" s="39"/>
-      <c r="E89" s="40"/>
+      <c r="E89" s="38"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
@@ -10485,7 +10495,7 @@
       </c>
       <c r="B90" s="39"/>
       <c r="D90" s="39"/>
-      <c r="E90" s="40"/>
+      <c r="E90" s="38"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
@@ -10493,7 +10503,7 @@
       </c>
       <c r="B91" s="39"/>
       <c r="D91" s="39"/>
-      <c r="E91" s="40"/>
+      <c r="E91" s="38"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
@@ -10501,7 +10511,7 @@
       </c>
       <c r="B92" s="39"/>
       <c r="D92" s="39"/>
-      <c r="E92" s="40"/>
+      <c r="E92" s="38"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
@@ -10509,7 +10519,7 @@
       </c>
       <c r="B93" s="39"/>
       <c r="D93" s="39"/>
-      <c r="E93" s="40"/>
+      <c r="E93" s="38"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
@@ -10517,7 +10527,7 @@
       </c>
       <c r="B94" s="39"/>
       <c r="D94" s="39"/>
-      <c r="E94" s="40"/>
+      <c r="E94" s="38"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
@@ -10525,7 +10535,7 @@
       </c>
       <c r="B95" s="39"/>
       <c r="D95" s="39"/>
-      <c r="E95" s="40"/>
+      <c r="E95" s="38"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
@@ -10533,7 +10543,7 @@
       </c>
       <c r="B96" s="39"/>
       <c r="D96" s="39"/>
-      <c r="E96" s="40"/>
+      <c r="E96" s="38"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
@@ -10541,7 +10551,7 @@
       </c>
       <c r="B97" s="39"/>
       <c r="D97" s="39"/>
-      <c r="E97" s="40"/>
+      <c r="E97" s="38"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
@@ -10549,7 +10559,7 @@
       </c>
       <c r="B98" s="39"/>
       <c r="D98" s="39"/>
-      <c r="E98" s="40"/>
+      <c r="E98" s="38"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
@@ -10557,7 +10567,7 @@
       </c>
       <c r="B99" s="39"/>
       <c r="D99" s="39"/>
-      <c r="E99" s="40"/>
+      <c r="E99" s="38"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
@@ -10565,7 +10575,7 @@
       </c>
       <c r="B100" s="39"/>
       <c r="D100" s="39"/>
-      <c r="E100" s="40"/>
+      <c r="E100" s="38"/>
     </row>
   </sheetData>
   <dataValidations count="10">
@@ -10632,7 +10642,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>

</xml_diff>

<commit_message>
Added Customers. Need to associate with Orders and Create HashMap.
</commit_message>
<xml_diff>
--- a/P11/Scrum_MICE_Sprint_5.xlsx
+++ b/P11/Scrum_MICE_Sprint_5.xlsx
@@ -1206,10 +1206,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822456753887466"/>
-          <c:y val="0.161896356071113"/>
-          <c:w val="0.884281521263973"/>
-          <c:h val="0.635607111335267"/>
+          <c:x val="0.0822508118910817"/>
+          <c:y val="0.161916771752837"/>
+          <c:w val="0.884211841119161"/>
+          <c:h val="0.635561160151324"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1318,11 +1318,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="3042615"/>
-        <c:axId val="37887512"/>
+        <c:axId val="36277787"/>
+        <c:axId val="67756759"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3042615"/>
+        <c:axId val="36277787"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1389,12 +1389,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37887512"/>
+        <c:crossAx val="67756759"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37887512"/>
+        <c:axId val="67756759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1469,7 +1469,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3042615"/>
+        <c:crossAx val="36277787"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1624,11 +1624,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="91226596"/>
-        <c:axId val="5972716"/>
+        <c:axId val="96673620"/>
+        <c:axId val="81209800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91226596"/>
+        <c:axId val="96673620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1693,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5972716"/>
+        <c:crossAx val="81209800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1701,7 +1701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5972716"/>
+        <c:axId val="81209800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,7 +1775,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91226596"/>
+        <c:crossAx val="96673620"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1930,11 +1930,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="15209356"/>
-        <c:axId val="67439798"/>
+        <c:axId val="99060412"/>
+        <c:axId val="92184231"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15209356"/>
+        <c:axId val="99060412"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +1999,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67439798"/>
+        <c:crossAx val="92184231"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2007,7 +2007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67439798"/>
+        <c:axId val="92184231"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2081,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15209356"/>
+        <c:crossAx val="99060412"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2236,11 +2236,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="26623412"/>
-        <c:axId val="82430155"/>
+        <c:axId val="46256996"/>
+        <c:axId val="87072029"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26623412"/>
+        <c:axId val="46256996"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2305,7 +2305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82430155"/>
+        <c:crossAx val="87072029"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2313,7 +2313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82430155"/>
+        <c:axId val="87072029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2387,7 +2387,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26623412"/>
+        <c:crossAx val="46256996"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2542,11 +2542,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="23676919"/>
-        <c:axId val="26832876"/>
+        <c:axId val="72431032"/>
+        <c:axId val="47087064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="23676919"/>
+        <c:axId val="72431032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,7 +2611,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26832876"/>
+        <c:crossAx val="47087064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2619,7 +2619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26832876"/>
+        <c:axId val="47087064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2693,7 +2693,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23676919"/>
+        <c:crossAx val="72431032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2833,7 +2833,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2848,11 +2848,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="30487926"/>
-        <c:axId val="62234585"/>
+        <c:axId val="98595829"/>
+        <c:axId val="33754770"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30487926"/>
+        <c:axId val="98595829"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,7 +2917,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62234585"/>
+        <c:crossAx val="33754770"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2925,7 +2925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62234585"/>
+        <c:axId val="33754770"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2999,7 +2999,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30487926"/>
+        <c:crossAx val="98595829"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3154,11 +3154,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="71479420"/>
-        <c:axId val="67462817"/>
+        <c:axId val="83748132"/>
+        <c:axId val="38208832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71479420"/>
+        <c:axId val="83748132"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3223,7 +3223,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67462817"/>
+        <c:crossAx val="38208832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3231,7 +3231,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67462817"/>
+        <c:axId val="38208832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3305,7 +3305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71479420"/>
+        <c:crossAx val="83748132"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3343,9 +3343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3201840</xdr:colOff>
+      <xdr:colOff>3201480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3353,8 +3353,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9116280" y="268200"/>
-        <a:ext cx="5764320" cy="2854800"/>
+        <a:off x="9115560" y="268200"/>
+        <a:ext cx="5763960" cy="2854440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3378,9 +3378,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3388,8 +3388,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3413,9 +3413,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3423,8 +3423,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3448,9 +3448,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3458,8 +3458,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3483,9 +3483,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3493,8 +3493,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3518,9 +3518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3528,8 +3528,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3553,9 +3553,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3563,8 +3563,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3596,7 +3596,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.57"/>
@@ -5697,7 +5697,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6679,7 +6679,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7656,7 +7656,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8651,7 +8651,7 @@
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9630,10 +9630,10 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9831,11 +9831,11 @@
       </c>
       <c r="B14" s="28" t="n">
         <f aca="false">B13-C14</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="28" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
@@ -9922,7 +9922,7 @@
         <v>95</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10642,7 +10642,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>

</xml_diff>

<commit_message>
Orders now associated with Customers. Updated backlog SS.
</commit_message>
<xml_diff>
--- a/P11/Scrum_MICE_Sprint_5.xlsx
+++ b/P11/Scrum_MICE_Sprint_5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="220">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -1206,10 +1206,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822508118910817"/>
-          <c:y val="0.161916771752837"/>
-          <c:w val="0.884211841119161"/>
-          <c:h val="0.635561160151324"/>
+          <c:x val="0.0822559490350384"/>
+          <c:y val="0.161937192584185"/>
+          <c:w val="0.884142152270314"/>
+          <c:h val="0.635515197376718"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1308,21 +1308,21 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="36277787"/>
-        <c:axId val="67756759"/>
+        <c:axId val="68995855"/>
+        <c:axId val="24404820"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="36277787"/>
+        <c:axId val="68995855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1389,12 +1389,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67756759"/>
+        <c:crossAx val="24404820"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67756759"/>
+        <c:axId val="24404820"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1469,7 +1469,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36277787"/>
+        <c:crossAx val="68995855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1624,11 +1624,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="96673620"/>
-        <c:axId val="81209800"/>
+        <c:axId val="20640754"/>
+        <c:axId val="38316580"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96673620"/>
+        <c:axId val="20640754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1693,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81209800"/>
+        <c:crossAx val="38316580"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1701,7 +1701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81209800"/>
+        <c:axId val="38316580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,7 +1775,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96673620"/>
+        <c:crossAx val="20640754"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1930,11 +1930,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="99060412"/>
-        <c:axId val="92184231"/>
+        <c:axId val="11809423"/>
+        <c:axId val="27304714"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99060412"/>
+        <c:axId val="11809423"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +1999,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92184231"/>
+        <c:crossAx val="27304714"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2007,7 +2007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92184231"/>
+        <c:axId val="27304714"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2081,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99060412"/>
+        <c:crossAx val="11809423"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2236,11 +2236,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="46256996"/>
-        <c:axId val="87072029"/>
+        <c:axId val="52412178"/>
+        <c:axId val="91575281"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46256996"/>
+        <c:axId val="52412178"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2305,7 +2305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87072029"/>
+        <c:crossAx val="91575281"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2313,7 +2313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87072029"/>
+        <c:axId val="91575281"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2387,7 +2387,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46256996"/>
+        <c:crossAx val="52412178"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2542,11 +2542,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="72431032"/>
-        <c:axId val="47087064"/>
+        <c:axId val="81170881"/>
+        <c:axId val="55158002"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72431032"/>
+        <c:axId val="81170881"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,7 +2611,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47087064"/>
+        <c:crossAx val="55158002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2619,7 +2619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47087064"/>
+        <c:axId val="55158002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2693,7 +2693,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72431032"/>
+        <c:crossAx val="81170881"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2833,7 +2833,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2848,11 +2848,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="98595829"/>
-        <c:axId val="33754770"/>
+        <c:axId val="33505747"/>
+        <c:axId val="93747143"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98595829"/>
+        <c:axId val="33505747"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,7 +2917,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33754770"/>
+        <c:crossAx val="93747143"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2925,7 +2925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33754770"/>
+        <c:axId val="93747143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2999,7 +2999,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98595829"/>
+        <c:crossAx val="33505747"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3154,11 +3154,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="83748132"/>
-        <c:axId val="38208832"/>
+        <c:axId val="46370848"/>
+        <c:axId val="52750518"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83748132"/>
+        <c:axId val="46370848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3223,7 +3223,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38208832"/>
+        <c:crossAx val="52750518"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3231,7 +3231,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38208832"/>
+        <c:axId val="52750518"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3305,7 +3305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83748132"/>
+        <c:crossAx val="46370848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3343,9 +3343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3201480</xdr:colOff>
+      <xdr:colOff>3201120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3353,8 +3353,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9115560" y="268200"/>
-        <a:ext cx="5763960" cy="2854440"/>
+        <a:off x="9114840" y="268200"/>
+        <a:ext cx="5763600" cy="2854080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3378,9 +3378,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3388,8 +3388,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3413,9 +3413,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3423,8 +3423,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3448,9 +3448,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3458,8 +3458,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3483,9 +3483,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3493,8 +3493,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3518,9 +3518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3528,8 +3528,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3553,9 +3553,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3563,8 +3563,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3585,8 +3585,8 @@
   </sheetPr>
   <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I38" activeCellId="0" sqref="I38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3834,11 +3834,11 @@
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">B16-C17</f>
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C17" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$110,"Finished in Sprint 5")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="3"/>
@@ -3854,7 +3854,7 @@
       </c>
       <c r="B18" s="3" t="n">
         <f aca="false">B17-C18</f>
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$110,"Finished in Sprint 6")</f>
@@ -4428,7 +4428,9 @@
       <c r="F38" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="G38" s="26"/>
+      <c r="G38" s="18" t="s">
+        <v>78</v>
+      </c>
       <c r="H38" s="24" t="s">
         <v>32</v>
       </c>
@@ -4459,7 +4461,9 @@
       <c r="F39" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="G39" s="26"/>
+      <c r="G39" s="18" t="s">
+        <v>78</v>
+      </c>
       <c r="H39" s="24" t="s">
         <v>57</v>
       </c>
@@ -4490,7 +4494,9 @@
       <c r="F40" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="G40" s="26"/>
+      <c r="G40" s="18" t="s">
+        <v>78</v>
+      </c>
       <c r="H40" s="24" t="s">
         <v>79</v>
       </c>
@@ -4521,7 +4527,9 @@
       <c r="F41" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="G41" s="26"/>
+      <c r="G41" s="18" t="s">
+        <v>78</v>
+      </c>
       <c r="H41" s="24" t="s">
         <v>32</v>
       </c>
@@ -5670,7 +5678,7 @@
       <formula1>"1,2,3,4,5,6"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" errorTitle="Wrong Value" operator="equal" prompt="Leave blank initially (hint: Use the Delete key)&#10;Select &quot;In Work&quot; when you begin designing and coding this feature.&#10;Select &quot;In Test&quot; when this feature is fully coded and you are testing it.&#10;Select  Finished ONLY when the feature works well and is READY TO" promptTitle="Implementation Status" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G24:G37 G69:G104" type="list">
+    <dataValidation allowBlank="true" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" errorTitle="Wrong Value" operator="equal" prompt="Leave blank initially (hint: Use the Delete key)&#10;Select &quot;In Work&quot; when you begin designing and coding this feature.&#10;Select &quot;In Test&quot; when this feature is fully coded and you are testing it.&#10;Select  Finished ONLY when the feature works well and is READY TO" promptTitle="Implementation Status" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G24:G41 G69:G104" type="list">
       <formula1>"In Work,In Test,Finished in Sprint 1,Finished in Sprint 2,Finished in Sprint 3,Finished in Sprint 4,Finished in Sprint 5,Finished in Sprint 6"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5697,7 +5705,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6679,7 +6687,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7656,7 +7664,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8651,7 +8659,7 @@
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9629,11 +9637,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9831,11 +9839,11 @@
       </c>
       <c r="B14" s="28" t="n">
         <f aca="false">B13-C14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="28" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
@@ -9936,7 +9944,7 @@
         <v>99</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10642,7 +10650,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>

</xml_diff>